<commit_message>
Update CONVERSION abs. chillers
Due to conflict issues with commit #3579
</commit_message>
<xml_diff>
--- a/cea/databases/DE/components/CONVERSION.xlsx
+++ b/cea/databases/DE/components/CONVERSION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\CityEnergyAnalyst\cea\databases\DE\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8CEF1B-A8E7-41F1-982E-5A9B70AB2C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC5228D-93AA-466A-9986-2AF12E91CFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="993" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="993" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHOTOVOLTAIC_PANELS" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="263">
   <si>
     <t>Description</t>
   </si>
@@ -837,6 +837,9 @@
   </si>
   <si>
     <t>1,176 EUR 2022 = 1 USD 2025</t>
+  </si>
+  <si>
+    <t>ASHRAE 90.1/2019 - minimum efficiency rating at full load; https://www.esmagazine.com/articles/82307-basics-for-absorption-chillers - capacity-specific mass-flow rates</t>
   </si>
 </sst>
 </file>
@@ -930,7 +933,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1090,6 +1093,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="59"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1098,7 +1110,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1145,9 +1157,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1243,10 +1252,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1718,85 +1724,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AA1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2753,67 +2759,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2985,73 +2991,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="V1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="W1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3092,7 +3098,7 @@
       <c r="L2" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="2">
@@ -3121,7 +3127,7 @@
         <v>5</v>
       </c>
       <c r="V2" s="14"/>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3162,7 +3168,7 @@
       <c r="L3" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="2">
@@ -3191,7 +3197,7 @@
         <v>5</v>
       </c>
       <c r="V3" s="14"/>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3232,7 +3238,7 @@
       <c r="L4" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N4" s="2">
@@ -3261,7 +3267,7 @@
         <v>6</v>
       </c>
       <c r="V4" s="14"/>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3302,7 +3308,7 @@
       <c r="L5" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N5" s="2">
@@ -3331,7 +3337,7 @@
         <v>6</v>
       </c>
       <c r="V5" s="14"/>
-      <c r="W5" s="27" t="s">
+      <c r="W5" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3372,7 +3378,7 @@
       <c r="L6" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N6" s="2">
@@ -3401,7 +3407,7 @@
         <v>6</v>
       </c>
       <c r="V6" s="14"/>
-      <c r="W6" s="27" t="s">
+      <c r="W6" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3442,7 +3448,7 @@
       <c r="L7" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N7" s="2">
@@ -3471,7 +3477,7 @@
         <v>6</v>
       </c>
       <c r="V7" s="14"/>
-      <c r="W7" s="27" t="s">
+      <c r="W7" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3512,7 +3518,7 @@
       <c r="L8" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N8" s="2">
@@ -3541,7 +3547,7 @@
         <v>6</v>
       </c>
       <c r="V8" s="14"/>
-      <c r="W8" s="27" t="s">
+      <c r="W8" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3582,7 +3588,7 @@
       <c r="L9" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="2">
@@ -3611,7 +3617,7 @@
         <v>6</v>
       </c>
       <c r="V9" s="14"/>
-      <c r="W9" s="27" t="s">
+      <c r="W9" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3652,7 +3658,7 @@
       <c r="L10" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N10" s="2">
@@ -3681,7 +3687,7 @@
         <v>6</v>
       </c>
       <c r="V10" s="14"/>
-      <c r="W10" s="27" t="s">
+      <c r="W10" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3722,7 +3728,7 @@
       <c r="L11" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N11" s="2">
@@ -3751,7 +3757,7 @@
         <v>6</v>
       </c>
       <c r="V11" s="14"/>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="26" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4416,82 +4422,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5092,73 +5098,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="V1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="W1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
@@ -5231,7 +5237,7 @@
       <c r="V2" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="26" t="s">
         <v>223</v>
       </c>
     </row>
@@ -5303,7 +5309,7 @@
       <c r="V3" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="26" t="s">
         <v>223</v>
       </c>
     </row>
@@ -5376,13 +5382,13 @@
       <c r="V4" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="26" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="U7" s="42"/>
+      <c r="A7" s="41"/>
+      <c r="U7" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5408,54 +5414,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5794,103 +5800,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="36" t="s">
+      <c r="W1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AA1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AB1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="36" t="s">
+      <c r="AC1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="36" t="s">
+      <c r="AD1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="36" t="s">
+      <c r="AE1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="36" t="s">
+      <c r="AF1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="36" t="s">
+      <c r="AG1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
@@ -6129,49 +6135,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
@@ -6235,7 +6241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -6343,7 +6349,7 @@
       <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <v>0.93</v>
       </c>
       <c r="I2" s="2">
@@ -6409,7 +6415,7 @@
       <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="21">
         <v>0.95</v>
       </c>
       <c r="I3" s="2">
@@ -6475,7 +6481,7 @@
       <c r="G4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <v>0.95</v>
       </c>
       <c r="I4" s="2">
@@ -6541,7 +6547,7 @@
       <c r="G5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="21">
         <v>0.95</v>
       </c>
       <c r="I5" s="2">
@@ -6607,7 +6613,7 @@
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <v>0.92</v>
       </c>
       <c r="I6" s="2">
@@ -6676,7 +6682,7 @@
       <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>0.93</v>
       </c>
       <c r="I7" s="2">
@@ -6745,7 +6751,7 @@
       <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <v>0.93</v>
       </c>
       <c r="I8" s="2">
@@ -6814,7 +6820,7 @@
       <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
         <v>0.93</v>
       </c>
       <c r="I9" s="2">
@@ -6829,7 +6835,7 @@
       <c r="L9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="53">
+      <c r="M9" s="44">
         <v>0</v>
       </c>
       <c r="N9">
@@ -6883,7 +6889,7 @@
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <v>0.93</v>
       </c>
       <c r="I10" s="2">
@@ -6952,7 +6958,7 @@
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="21">
         <v>0.95</v>
       </c>
       <c r="I11" s="2">
@@ -7021,7 +7027,7 @@
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
         <v>0.95</v>
       </c>
       <c r="I12" s="2">
@@ -7072,7 +7078,7 @@
       <c r="A13" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="9" t="s">
         <v>225</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -7090,7 +7096,7 @@
       <c r="G13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="21">
         <v>0.95</v>
       </c>
       <c r="I13" s="2">
@@ -7138,28 +7144,28 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="45" t="s">
         <v>237</v>
       </c>
       <c r="D14" t="s">
         <v>246</v>
       </c>
-      <c r="E14" s="49">
-        <v>1</v>
-      </c>
-      <c r="F14" s="49">
+      <c r="E14" s="48">
+        <v>1</v>
+      </c>
+      <c r="F14" s="48">
         <v>10000000000</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="49">
         <v>1</v>
       </c>
       <c r="I14" s="2">
@@ -7207,28 +7213,28 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="45" t="s">
         <v>238</v>
       </c>
       <c r="D15" t="s">
         <v>247</v>
       </c>
-      <c r="E15" s="49">
-        <v>1</v>
-      </c>
-      <c r="F15" s="49">
+      <c r="E15" s="48">
+        <v>1</v>
+      </c>
+      <c r="F15" s="48">
         <v>30000</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="50">
+      <c r="H15" s="49">
         <v>0.94</v>
       </c>
       <c r="I15" s="2">
@@ -7276,28 +7282,28 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="45" t="s">
         <v>238</v>
       </c>
       <c r="D16" t="s">
         <v>247</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E16" s="48">
         <v>30000</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="48">
         <v>60000</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="50">
+      <c r="H16" s="49">
         <v>0.94</v>
       </c>
       <c r="I16" s="2">
@@ -7345,28 +7351,28 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="45" t="s">
         <v>238</v>
       </c>
       <c r="D17" t="s">
         <v>247</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="48">
         <v>60000</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="48">
         <v>230000</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="50">
+      <c r="H17" s="49">
         <v>0.94</v>
       </c>
       <c r="I17" s="2">
@@ -7414,28 +7420,28 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="45" t="s">
         <v>240</v>
       </c>
       <c r="D18" t="s">
         <v>248</v>
       </c>
-      <c r="E18" s="49">
-        <v>1</v>
-      </c>
-      <c r="F18" s="49">
+      <c r="E18" s="48">
+        <v>1</v>
+      </c>
+      <c r="F18" s="48">
         <v>20000</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="50">
         <v>0.9</v>
       </c>
       <c r="I18" s="2">
@@ -7483,28 +7489,28 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="45" t="s">
         <v>240</v>
       </c>
       <c r="D19" t="s">
         <v>248</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="48">
         <v>20000</v>
       </c>
-      <c r="F19" s="49">
+      <c r="F19" s="48">
         <v>60000</v>
       </c>
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H19" s="50">
         <v>0.85</v>
       </c>
       <c r="I19" s="2">
@@ -7552,28 +7558,28 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="45" t="s">
         <v>240</v>
       </c>
       <c r="D20" t="s">
         <v>248</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="48">
         <v>60000</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="48">
         <v>1000000000</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="50">
         <v>0.81</v>
       </c>
       <c r="I20" s="2">
@@ -7604,13 +7610,13 @@
       <c r="Q20" s="2">
         <v>0</v>
       </c>
-      <c r="R20" s="45">
+      <c r="R20" s="44">
         <v>20</v>
       </c>
-      <c r="S20" s="45">
+      <c r="S20" s="44">
         <v>6</v>
       </c>
-      <c r="T20" s="45">
+      <c r="T20" s="44">
         <v>5</v>
       </c>
       <c r="U20" t="s">
@@ -7651,73 +7657,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="39" t="s">
+      <c r="G1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>127</v>
       </c>
     </row>
@@ -7743,16 +7749,16 @@
       <c r="G2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>0.4</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I2" s="31">
         <v>0.47</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="33">
         <v>380</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2" s="32">
         <v>100</v>
       </c>
       <c r="L2" s="12">
@@ -7788,7 +7794,7 @@
       <c r="V2" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -7796,31 +7802,31 @@
       <c r="A3" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>162</v>
       </c>
       <c r="E3" s="17">
         <v>2600000</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>3500000</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>0.43</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="28">
         <v>0.44</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="34">
         <v>380</v>
       </c>
       <c r="K3" s="12">
@@ -7859,7 +7865,7 @@
       <c r="V3" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="W3" s="31" t="s">
+      <c r="W3" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -7876,22 +7882,22 @@
       <c r="D4" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>3500000</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <v>10000000</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="29">
         <v>0.45500000000000002</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="29">
         <v>0.43</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="33">
         <v>380</v>
       </c>
       <c r="K4" s="11">
@@ -7930,7 +7936,7 @@
       <c r="V4" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="W4" s="31" t="s">
+      <c r="W4" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -7947,22 +7953,22 @@
       <c r="D5" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>180000</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>280000</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <v>0.35</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>0.39</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="33">
         <v>380</v>
       </c>
       <c r="K5" s="11">
@@ -8001,7 +8007,7 @@
       <c r="V5" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="W5" s="31" t="s">
+      <c r="W5" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -8018,22 +8024,22 @@
       <c r="D6" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>280000</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>900000</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="29">
         <v>0.39</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="29">
         <v>0.4</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="33">
         <v>380</v>
       </c>
       <c r="K6" s="11">
@@ -8072,7 +8078,7 @@
       <c r="V6" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="W6" s="31" t="s">
+      <c r="W6" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -8089,22 +8095,22 @@
       <c r="D7" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>900000</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>2600000</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="29">
         <v>0.42</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>0.41</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="33">
         <v>380</v>
       </c>
       <c r="K7" s="11">
@@ -8143,7 +8149,7 @@
       <c r="V7" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="W7" s="31" t="s">
+      <c r="W7" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -8160,22 +8166,22 @@
       <c r="D8" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>1000000</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>5000000</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="29">
         <v>0.15</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>0.65</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="33">
         <v>380</v>
       </c>
       <c r="K8" s="11">
@@ -8190,7 +8196,7 @@
       <c r="N8" s="11">
         <v>0</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="25">
         <v>0.74299999999999999</v>
       </c>
       <c r="P8" s="11">
@@ -8214,7 +8220,7 @@
       <c r="V8" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W8" s="27" t="s">
+      <c r="W8" s="26" t="s">
         <v>179</v>
       </c>
     </row>
@@ -8231,22 +8237,22 @@
       <c r="D9" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>5000000</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>50000000</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="29">
         <v>0.17</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>0.67</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="33">
         <v>380</v>
       </c>
       <c r="K9" s="11">
@@ -8285,7 +8291,7 @@
       <c r="V9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W9" s="27" t="s">
+      <c r="W9" s="26" t="s">
         <v>179</v>
       </c>
     </row>
@@ -8302,22 +8308,22 @@
       <c r="D10" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>1000000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>50000000</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="29">
         <v>0.18</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="29">
         <v>0.8</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="33">
         <v>380</v>
       </c>
       <c r="K10" s="11">
@@ -8332,7 +8338,7 @@
       <c r="N10" s="11">
         <v>0</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="25">
         <v>0.74299999999999999</v>
       </c>
       <c r="P10" s="11">
@@ -8356,7 +8362,7 @@
       <c r="V10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W10" s="27" t="s">
+      <c r="W10" s="26" t="s">
         <v>179</v>
       </c>
     </row>
@@ -8373,22 +8379,22 @@
       <c r="D11" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <v>30000000</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>150000000</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="29">
         <v>0.62</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="29">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="33">
         <v>380</v>
       </c>
       <c r="K11" s="11">
@@ -8428,7 +8434,7 @@
       <c r="V11" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="26" t="s">
         <v>183</v>
       </c>
     </row>
@@ -8464,67 +8470,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
@@ -8591,7 +8597,7 @@
       <c r="T2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="U2" s="26" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8657,7 +8663,7 @@
       <c r="T3" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="U3" s="26" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8671,10 +8677,10 @@
       <c r="C4" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>100000</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>10000000000</v>
       </c>
       <c r="F4" s="12" t="s">
@@ -8724,7 +8730,7 @@
       <c r="T4" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="26" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8813,70 +8819,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>127</v>
       </c>
     </row>
@@ -8958,7 +8964,7 @@
       <c r="C3" s="11">
         <v>0.4</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="17">
@@ -9028,7 +9034,7 @@
       <c r="C4" s="11">
         <v>0.4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E4" s="17">
@@ -9098,7 +9104,7 @@
       <c r="C5" s="11">
         <v>0.4</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E5" s="17">
@@ -9168,7 +9174,7 @@
       <c r="C6" s="11">
         <v>0.4</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="17">
@@ -9238,7 +9244,7 @@
       <c r="C7" s="11">
         <v>0.4</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E7" s="17">
@@ -9314,8 +9320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2:AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9524,13 +9530,13 @@
         <v>1.5</v>
       </c>
       <c r="AE2" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>128</v>
+        <v>3.23</v>
+      </c>
+      <c r="AF2" s="14">
+        <v>2.14</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -9627,10 +9633,10 @@
       <c r="AE3" s="2">
         <v>81</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF3" s="14">
         <v>33</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AG3" s="11" t="s">
         <v>128</v>
       </c>
     </row>
@@ -9725,14 +9731,14 @@
       <c r="AD4" s="2">
         <v>1.5</v>
       </c>
-      <c r="AE4" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>128</v>
+      <c r="AE4" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="AF4" s="51">
+        <v>2.5</v>
+      </c>
+      <c r="AG4" s="11" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
@@ -9829,10 +9835,10 @@
       <c r="AE5" s="2">
         <v>68</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AF5" s="14">
         <v>14</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AG5" s="11" t="s">
         <v>128</v>
       </c>
     </row>
@@ -9927,14 +9933,14 @@
       <c r="AD6" s="2">
         <v>4.38</v>
       </c>
-      <c r="AE6" s="2">
-        <v>68</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>14</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>128</v>
+      <c r="AE6" s="14">
+        <v>646</v>
+      </c>
+      <c r="AF6" s="51">
+        <v>431</v>
+      </c>
+      <c r="AG6" s="11" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
@@ -10031,10 +10037,10 @@
       <c r="AE7" s="2">
         <v>62</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AF7" s="14">
         <v>10</v>
       </c>
-      <c r="AG7" s="18"/>
+      <c r="AG7" s="26"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -10069,70 +10075,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="V1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
@@ -10155,7 +10161,7 @@
       <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="19">
         <v>1.26E-2</v>
       </c>
       <c r="H2" s="2">
@@ -10223,7 +10229,7 @@
       <c r="F3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>1.26E-2</v>
       </c>
       <c r="H3" s="12">
@@ -10291,7 +10297,7 @@
       <c r="F4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="19">
         <v>3.15E-2</v>
       </c>
       <c r="H4" s="12">
@@ -10359,7 +10365,7 @@
       <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>3.15E-2</v>
       </c>
       <c r="H5" s="11">
@@ -10377,7 +10383,7 @@
       <c r="L5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="18">
         <v>1457.3</v>
       </c>
       <c r="N5" s="2">
@@ -10422,7 +10428,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="V7" s="21"/>
+      <c r="V7" s="20"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>